<commit_message>
Complete Authorization and Navigation tests
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <s:workbookPr/>
   <s:bookViews>
     <s:workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240"/>
@@ -2273,11 +2273,20 @@
   <s:si>
     <s:t>TC-LOGOUT-02</s:t>
   </s:si>
+  <s:si>
+    <s:t>1. Нажать кнопку "гамбургер" для открытия бокового меню.
+2. Проверить состояние пункта "Main".
+3. Проверить состояние пункта "News".
+4. Проверить состояние пункта "About".
+5. Нажать пункт "News".
+6. Вернуться в раздел "Main"
+7. Нажать пункт "About".</s:t>
+  </s:si>
 </s:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<s:styleSheet xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:vyd="http://volga.yandex.com/schemas/document/model">
+<s:styleSheet xmlns:vyd="http://volga.yandex.com/schemas/document/model" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:numFmts count="0"/>
   <s:fonts count="10">
     <s:font>
@@ -3273,7 +3282,7 @@
       <s:c r="K16" s="37"/>
       <s:c r="L16" s="37"/>
     </s:row>
-    <s:row r="17" ht="90">
+    <s:row r="17" ht="92.25">
       <s:c r="A17" s="35" t="s">
         <s:v>91</s:v>
       </s:c>
@@ -3284,7 +3293,7 @@
         <s:v>495</s:v>
       </s:c>
       <s:c r="D17" s="35" t="s">
-        <s:v>521</s:v>
+        <s:v>644</s:v>
       </s:c>
       <s:c r="E17" s="35" t="s">
         <s:v>493</s:v>

</xml_diff>

<commit_message>
Optimized Allure.step and timings
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr/>
   <s:bookViews>
     <s:workbookView xWindow="3160" yWindow="2260" windowWidth="28240" windowHeight="17240"/>
@@ -2282,13 +2282,64 @@
 6. Вернуться в раздел "Main"
 7. Нажать пункт "About".</s:t>
   </s:si>
+  <s:si>
+    <s:t>1. Нажать на верхней панели кнопку перехода в "Quotes".
+2. Выбрать цитату.
+3. Нажать стрелку у одной из цитат.
+4. Еще раз нажать стрелку у той же цитаты.</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Нажать на верхней панели кнопку перехода в "Quotes".
+2. Нажать стрелку у одной из цитат.
+3. Еще раз нажать стрелку у той же цитаты.</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Открывается вкладка Quotes с заголовком "Love is all".
+2. Под цитатой раскрывается отзыв пользователя.
+3. Отзыв скрывается.</s:t>
+  </s:si>
+  <s:si>
+    <s:t>Полный E2E сценарий редактирования новости</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Перейти к редактированию существующей новости.
+2. Проверить, что поля предзаполнены валидными данными
+3. Проверить состояние чекбокса "Active"
+</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Перейти к редактированию существующей новости.
+2. Проверить, что поля предзаполнены валидными данными
+3. Проверить состояние чекбокса "Active"
+4. Изменить поле "Title"</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Перейти к редактированию существующей новости.
+2. Проверить, что поля предзаполнены валидными данными
+3. Проверить состояние чекбокса "Active"
+4. Изменить поле "Title"
+5. Проверить, что поле "Title" в новости обновилось</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Все поля формы предзаполнены данными новости.</s:t>
+  </s:si>
+  <s:si>
+    <s:t>1. Все поля формы предзаполнены данными новости.
+2. Новость обновилась и отображается в списке новостей</s:t>
+  </s:si>
+  <s:si>
+    <s:t>Полный E2E сценарий редактирования новости с проверкой предзаполнения полей</s:t>
+  </s:si>
+  <s:si>
+    <s:t>Полный E2E сценарий удаления новости</s:t>
+  </s:si>
 </s:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<s:styleSheet xmlns:vyd="http://volga.yandex.com/schemas/document/model" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<s:styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:vyd="http://volga.yandex.com/schemas/document/model" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:numFmts count="0"/>
-  <s:fonts count="10">
+  <s:fonts count="12">
     <s:font>
       <s:name val="Arial"/>
       <s:family val="2"/>
@@ -2331,8 +2382,16 @@
       <s:b val="1"/>
       <s:sz val="12"/>
     </s:font>
+    <s:font>
+      <s:name val="JetBrains Mono"/>
+      <s:color rgb="FFBCBEC4"/>
+    </s:font>
+    <s:font>
+      <s:name val="JetBrains Mono"/>
+      <s:color rgb="FF000000"/>
+    </s:font>
   </s:fonts>
-  <s:fills count="3">
+  <s:fills count="5">
     <s:fill>
       <s:patternFill patternType="none"/>
     </s:fill>
@@ -2342,6 +2401,17 @@
     <s:fill>
       <s:patternFill patternType="solid">
         <s:fgColor rgb="FFFFFFFF"/>
+      </s:patternFill>
+    </s:fill>
+    <s:fill>
+      <s:patternFill patternType="solid">
+        <s:fgColor rgb="FF1E1F22"/>
+      </s:patternFill>
+    </s:fill>
+    <s:fill>
+      <s:patternFill patternType="solid">
+        <s:fgColor rgb="FFFFFFFF"/>
+        <s:bgColor rgb="FFFFFFFF"/>
       </s:patternFill>
     </s:fill>
   </s:fills>
@@ -2390,7 +2460,7 @@
   <s:cellStyleXfs count="1">
     <s:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </s:cellStyleXfs>
-  <s:cellXfs count="43">
+  <s:cellXfs count="48">
     <s:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <s:xf fontId="1" fillId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <s:alignment horizontal="left" wrapText="0" vyd:clipText="0" mc:Ignorable="vyd"/>
@@ -2512,6 +2582,15 @@
       <s:alignment vertical="center" mc:Ignorable="vyd"/>
     </s:xf>
     <s:xf borderId="4" applyBorder="1" applyAlignment="1">
+      <s:alignment vertical="center" wrapText="1" vyd:clipText="0" mc:Ignorable="vyd"/>
+    </s:xf>
+    <s:xf fontId="10" fillId="3" applyFont="1" applyFill="1"/>
+    <s:xf fontId="10" fillId="4" applyFont="1" applyFill="1"/>
+    <s:xf fontId="11" fillId="4" applyFont="1" applyFill="1"/>
+    <s:xf fontId="11" fillId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <s:alignment vertical="center" mc:Ignorable="vyd"/>
+    </s:xf>
+    <s:xf fontId="11" fillId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <s:alignment vertical="center" wrapText="1" vyd:clipText="0" mc:Ignorable="vyd"/>
     </s:xf>
   </s:cellXfs>
@@ -4220,12 +4299,12 @@
         <s:v>46</s:v>
       </s:c>
     </s:row>
-    <s:row r="44" ht="68.25">
+    <s:row r="44" ht="69.75">
       <s:c r="A44" s="35" t="s">
         <s:v>239</s:v>
       </s:c>
-      <s:c r="B44" s="35" t="s">
-        <s:v>240</s:v>
+      <s:c r="B44" s="47" t="s">
+        <s:v>655</s:v>
       </s:c>
       <s:c r="C44" s="35" t="s">
         <s:v>149</s:v>
@@ -4947,10 +5026,10 @@
         <s:v>44</s:v>
       </s:c>
       <s:c r="J63" s="35" t="s">
-        <s:v>59</s:v>
+        <s:v>45</s:v>
       </s:c>
       <s:c r="K63" s="35" t="s">
-        <s:v>59</s:v>
+        <s:v>45</s:v>
       </s:c>
       <s:c r="L63" s="35" t="s">
         <s:v>510</s:v>
@@ -5086,24 +5165,24 @@
       <s:c r="K67" s="37"/>
       <s:c r="L67" s="37"/>
     </s:row>
-    <s:row r="68" ht="35.25">
+    <s:row r="68" ht="92.25">
       <s:c r="A68" s="35" t="s">
         <s:v>320</s:v>
       </s:c>
       <s:c r="B68" s="35" t="s">
-        <s:v>321</s:v>
+        <s:v>654</s:v>
       </s:c>
       <s:c r="C68" s="35" t="s">
         <s:v>322</s:v>
       </s:c>
       <s:c r="D68" s="35" t="s">
-        <s:v>323</s:v>
+        <s:v>651</s:v>
       </s:c>
       <s:c r="E68" s="35" t="s">
-        <s:v>324</s:v>
+        <s:v>653</s:v>
       </s:c>
       <s:c r="F68" s="35" t="s">
-        <s:v>324</s:v>
+        <s:v>653</s:v>
       </s:c>
       <s:c r="G68" s="35" t="s">
         <s:v>42</s:v>
@@ -5330,7 +5409,7 @@
       <s:c r="K74" s="37"/>
       <s:c r="L74" s="37"/>
     </s:row>
-    <s:row r="75" ht="68.25">
+    <s:row r="75" ht="69.75">
       <s:c r="A75" s="35" t="s">
         <s:v>352</s:v>
       </s:c>
@@ -5341,13 +5420,13 @@
         <s:v>169</s:v>
       </s:c>
       <s:c r="D75" s="35" t="s">
-        <s:v>354</s:v>
+        <s:v>646</s:v>
       </s:c>
       <s:c r="E75" s="35" t="s">
-        <s:v>355</s:v>
+        <s:v>647</s:v>
       </s:c>
       <s:c r="F75" s="35" t="s">
-        <s:v>355</s:v>
+        <s:v>647</s:v>
       </s:c>
       <s:c r="G75" s="35" t="s">
         <s:v>42</s:v>

</xml_diff>